<commit_message>
address mapping with MML, openEHR, HL7 2.5 and FHIR.
</commit_message>
<xml_diff>
--- a/mapping/mml_address_mapping.xlsx
+++ b/mapping/mml_address_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>Elements</t>
   </si>
@@ -109,14 +109,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>openEHR-EHR-CLUSTER-address-japan.v1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Address type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Unstructured address</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -150,6 +142,278 @@
   </si>
   <si>
     <t>country code</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.address-japan.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Address type(注)</t>
+    <rPh sb="13" eb="14">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>注</t>
+    <rPh sb="0" eb="1">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>Current or Temporary</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>mailing</t>
+  </si>
+  <si>
+    <t>Mailing</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>County of Origin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>temporary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>residential</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>business</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>correspondence</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Permanent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Legal address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Legal address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*country of origin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*birth</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Office</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Birth delivery location</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Birth delivery location(use for birth facility)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Residence at birth</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Resident for birth(use for residence at birth)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Resistry home</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*Bad address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MMLのaddressClass(HL7-0190)とそれに対応するArchetype table(*は拡張部分)</t>
+    <rPh sb="30" eb="32">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>カクチョウ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Representation code</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HL7-0190</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HL7 ver 2.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SAD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XAD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1(SAD)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4(state)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(未定義）</t>
+    <rPh sb="1" eb="4">
+      <t>ミテイギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6(country)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8(Other geographic designation)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10(Census tract)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>address valid period</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>valid from</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>valid to</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12(非推奨）</t>
+    <rPh sb="3" eb="6">
+      <t>ヒスイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HL7 FHIR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>use</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>city</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>state</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>zip</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>country</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>period</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HL7 FHIR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>work</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>temp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>old</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -157,7 +421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +434,15 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -220,7 +493,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,6 +504,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -548,15 +830,21 @@
     <col min="8" max="8" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -574,10 +862,19 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -588,11 +885,8 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -607,8 +901,14 @@
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -623,8 +923,17 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -637,8 +946,11 @@
         <v>11</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H6" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -654,10 +966,19 @@
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -673,13 +994,13 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -695,10 +1016,16 @@
       </c>
       <c r="F9" s="1"/>
       <c r="I9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -714,10 +1041,13 @@
       </c>
       <c r="F10" s="1"/>
       <c r="I10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -733,10 +1063,13 @@
       </c>
       <c r="F11" s="1"/>
       <c r="I11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -752,10 +1085,16 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -771,12 +1110,250 @@
       </c>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H14" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I15" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>104</v>
+      </c>
+      <c r="N19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="81" x14ac:dyDescent="0.15">
+      <c r="B28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="81" x14ac:dyDescent="0.15">
+      <c r="B29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="27" x14ac:dyDescent="0.15">
+      <c r="B30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="27" x14ac:dyDescent="0.15">
+      <c r="B31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
mml health insurance module
</commit_message>
<xml_diff>
--- a/mapping/mml_address_mapping.xlsx
+++ b/mapping/mml_address_mapping.xlsx
@@ -303,10 +303,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>HL7-0190</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HL7 ver 2.5</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -434,6 +430,10 @@
   </si>
   <si>
     <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*ValueはHL7-0190</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -830,7 +830,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -849,10 +849,10 @@
         <v>39</v>
       </c>
       <c r="L1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
@@ -876,13 +876,13 @@
         <v>31</v>
       </c>
       <c r="L2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" t="s">
         <v>81</v>
       </c>
-      <c r="M2" t="s">
-        <v>82</v>
-      </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -939,13 +939,13 @@
         <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M5">
         <v>7</v>
       </c>
       <c r="Q5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
@@ -961,8 +961,8 @@
         <v>11</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="H6" s="2" t="s">
-        <v>79</v>
+      <c r="K6" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
@@ -984,16 +984,16 @@
         <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
@@ -1018,7 +1018,7 @@
         <v>33</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
@@ -1040,13 +1040,13 @@
         <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M9">
         <v>3</v>
       </c>
       <c r="Q9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
@@ -1068,7 +1068,7 @@
         <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1093,7 +1093,7 @@
         <v>36</v>
       </c>
       <c r="J11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1121,7 +1121,7 @@
         <v>5</v>
       </c>
       <c r="Q12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
@@ -1146,26 +1146,26 @@
         <v>9</v>
       </c>
       <c r="Q13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="H14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M15">
         <v>13</v>
@@ -1176,10 +1176,10 @@
         <v>41</v>
       </c>
       <c r="I16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M16">
         <v>14</v>
@@ -1190,10 +1190,10 @@
         <v>77</v>
       </c>
       <c r="N17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.15">
@@ -1207,10 +1207,10 @@
         <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.15">
@@ -1224,10 +1224,10 @@
         <v>61</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.15">
@@ -1241,7 +1241,7 @@
         <v>65</v>
       </c>
       <c r="N20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.15">
@@ -1266,7 +1266,7 @@
         <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.15">
@@ -1291,7 +1291,7 @@
         <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.15">
@@ -1383,7 +1383,7 @@
         <v>76</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>